<commit_message>
add quantity to database
</commit_message>
<xml_diff>
--- a/Source_Data.xlsx
+++ b/Source_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document for Uni\year 3\dev Windows\myShop\MyShop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\source\repos\MyShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029F1768-1A09-4124-B0F7-FC0F2089788A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5050909D-660C-4C75-86B1-7A25133EED3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{DB7234D3-2EC2-4997-8AFC-75EF169559C6}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{DB7234D3-2EC2-4997-8AFC-75EF169559C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>STT</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>iporn</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -156,7 +159,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E435BCC4-08E0-4FB0-91D6-A3CEDCA6E993}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,10 +557,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7ECBFC6-17ED-48A3-9627-E724C929FEF1}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +568,7 @@
     <col min="2" max="2" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,8 +581,11 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -592,8 +598,11 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -606,8 +615,11 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -620,8 +632,11 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -634,8 +649,11 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -648,8 +666,11 @@
       <c r="D6" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -662,8 +683,11 @@
       <c r="D7" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -676,8 +700,11 @@
       <c r="D8" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -690,8 +717,11 @@
       <c r="D9" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -703,6 +733,9 @@
       </c>
       <c r="D10" s="1">
         <v>4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>